<commit_message>
Last update for rendu_p3_v2
</commit_message>
<xml_diff>
--- a/exercice3/Exercises_03_IR_indexing_weighting.xlsx
+++ b/exercice3/Exercises_03_IR_indexing_weighting.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <r>
       <rPr>
@@ -212,9 +212,6 @@
     <t>SMART ltc</t>
   </si>
   <si>
-    <t>SMART Information Retrieval System - Wikipedia</t>
-  </si>
-  <si>
     <t>d1</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
       </rPr>
       <t>1</t>
     </r>
-  </si>
-  <si>
-    <t>Okapi BM25 - Wikipedia</t>
   </si>
   <si>
     <r>
@@ -343,7 +337,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -362,12 +356,6 @@
       <name val="Calibri"/>
     </font>
     <font/>
-    <font>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -715,7 +703,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -798,34 +786,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2419350" cy="504825"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>15</xdr:row>
@@ -834,11 +794,11 @@
     <xdr:ext cx="2028825" cy="590550"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
+        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -890,7 +850,35 @@
     <xdr:ext cx="190500" cy="381000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2419350" cy="504825"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1711,9 +1699,7 @@
         <v>16</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="34" t="s">
-        <v>20</v>
-      </c>
+      <c r="J16" s="34"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1733,7 +1719,7 @@
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="31">
         <f t="shared" ref="C17:G17" si="2">C13/SQRT(SUMSQ($C13:$G13))</f>
@@ -1756,8 +1742,8 @@
         <v>0.2574943894</v>
       </c>
       <c r="H17" s="32">
-        <f t="shared" ref="H17:H18" si="4">SUM(C17:G17)</f>
-        <v>1.917681393</v>
+        <f t="shared" ref="H17:H18" si="4">SUMPRODUCT(C$6:G$6,C17:G17)</f>
+        <v>0.7609628699</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="2"/>
@@ -1781,7 +1767,7 @@
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="31">
         <f t="shared" ref="C18:G18" si="3">C14/SQRT(SUMSQ($C14:$G14))</f>
@@ -1805,7 +1791,7 @@
       </c>
       <c r="H18" s="32">
         <f t="shared" si="4"/>
-        <v>1.719297873</v>
+        <v>0.5236496403</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="2"/>
@@ -1858,7 +1844,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1887,7 +1873,7 @@
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="36">
         <f>(C4*(k_1+1))/(C4+k_1*(1-b+b*($H4/avdl)))</f>
@@ -1911,9 +1897,7 @@
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="34" t="s">
-        <v>25</v>
-      </c>
+      <c r="J21" s="34"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1934,7 +1918,7 @@
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="24"/>
       <c r="B22" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" s="36">
         <f>(C5*(k_1+1))/(C5+k_1*(1-b+b*($H5/avdl)))</f>
@@ -2008,7 +1992,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -2038,24 +2022,24 @@
       <c r="A25" s="18"/>
       <c r="B25" s="1"/>
       <c r="C25" s="37">
-        <f>LN(((N-C10+0.5)/(C10+0.5))+1)</f>
-        <v>4.557379522</v>
+        <f>LOG10((N-C10+0.5)/(C10+0.5))</f>
+        <v>1.974665181</v>
       </c>
       <c r="D25" s="37">
-        <f>LN(((N-D10+0.5)/(D10+0.5))+1)</f>
-        <v>3.670076327</v>
+        <f>LOG10((N-D10+0.5)/(D10+0.5))</f>
+        <v>1.582687093</v>
       </c>
       <c r="E25" s="37">
-        <f>LN(((N-E10+0.5)/(E10+0.5))+1)</f>
-        <v>4.557379522</v>
+        <f>LOG10((N-E10+0.5)/(E10+0.5))</f>
+        <v>1.974665181</v>
       </c>
       <c r="F25" s="37">
-        <f>LN(((N-F10+0.5)/(F10+0.5))+1)</f>
-        <v>3.710081662</v>
+        <f>LOG10((N-F10+0.5)/(F10+0.5))</f>
+        <v>1.600506163</v>
       </c>
       <c r="G25" s="37">
-        <f>LN(((N-G10+0.5)/(G10+0.5))+1)</f>
-        <v>1.385295859</v>
+        <f>LOG10((N-G10+0.5)/(G10+0.5))</f>
+        <v>0.4765429664</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -2108,7 +2092,7 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -2139,11 +2123,11 @@
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28" s="31">
         <f t="shared" ref="C28:G28" si="5">C21*C$25</f>
-        <v>5.135075518</v>
+        <v>2.224974852</v>
       </c>
       <c r="D28" s="31">
         <f t="shared" si="5"/>
@@ -2151,19 +2135,19 @@
       </c>
       <c r="E28" s="31">
         <f t="shared" si="5"/>
-        <v>5.135075518</v>
+        <v>2.224974852</v>
       </c>
       <c r="F28" s="31">
         <f t="shared" si="5"/>
-        <v>6.215843622</v>
+        <v>2.681476294</v>
       </c>
       <c r="G28" s="31">
         <f t="shared" si="5"/>
-        <v>2.398780708</v>
+        <v>0.8251826258</v>
       </c>
       <c r="H28" s="38">
-        <f t="shared" ref="H28:H29" si="7">SUM(C28:G28)</f>
-        <v>18.88477537</v>
+        <f t="shared" ref="H28:H29" si="7">SUMPRODUCT(C$6:G$6,C28:G28)</f>
+        <v>3.050157477</v>
       </c>
       <c r="I28" s="33"/>
       <c r="J28" s="2"/>
@@ -2187,19 +2171,19 @@
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29" s="31">
         <f t="shared" ref="C29:G29" si="6">C22*C$25</f>
-        <v>5.52409639</v>
+        <v>2.393533552</v>
       </c>
       <c r="D29" s="31">
         <f t="shared" si="6"/>
-        <v>6.31410981</v>
+        <v>2.722902526</v>
       </c>
       <c r="E29" s="31">
         <f t="shared" si="6"/>
-        <v>5.52409639</v>
+        <v>2.393533552</v>
       </c>
       <c r="F29" s="31">
         <f t="shared" si="6"/>
@@ -2211,7 +2195,7 @@
       </c>
       <c r="H29" s="38">
         <f t="shared" si="7"/>
-        <v>17.36230259</v>
+        <v>2.393533552</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -29430,14 +29414,10 @@
     <mergeCell ref="C24:G24"/>
     <mergeCell ref="C27:G27"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="J16"/>
-    <hyperlink r:id="rId2" ref="J21"/>
-  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.15748031496062992" footer="0.0" header="0.0" left="0.2362204724409449" right="0.2362204724409449" top="0.15748031496062992"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>